<commit_message>
commit survery data changes and readme file
</commit_message>
<xml_diff>
--- a/messy-project-directory/data/Survey_Data.xlsx
+++ b/messy-project-directory/data/Survey_Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trvrb/Documents/src/tfcb_2019/homeworks/homework01/messy-project-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haleydean/Documents/tfcb-homework01/messy-project-directory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A2EF31-99BB-1147-875E-0BF67F65B824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312D19E8-6F6F-7F40-BE08-5FA3A0BB4719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1400" windowWidth="25120" windowHeight="15580" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19100" windowHeight="15580" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="44">
   <si>
     <t>NA</t>
   </si>
@@ -140,6 +141,27 @@
   </si>
   <si>
     <t>gray cell means my measurement device wasn't calibrated correctly</t>
+  </si>
+  <si>
+    <t>Plot Number</t>
+  </si>
+  <si>
+    <t>Scale calibrated?</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>Weight (g)</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -149,7 +171,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -187,6 +209,11 @@
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -317,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,12 +361,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +829,7 @@
   <dimension ref="C3:AB28"/>
   <sheetViews>
     <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -903,294 +932,294 @@
       <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="16" t="s">
+      <c r="O7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C8" s="18">
+      <c r="C8" s="17">
         <v>41471</v>
       </c>
-      <c r="D8" s="16">
-        <v>2</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="17"/>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="18">
+      <c r="H8" s="17">
         <v>41505</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="5">
         <v>8</v>
       </c>
-      <c r="J8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="17">
+      <c r="J8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16">
         <v>52</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="18">
+      <c r="M8" s="17">
         <v>41590</v>
       </c>
-      <c r="N8" s="16">
+      <c r="N8" s="5">
         <v>9</v>
       </c>
-      <c r="O8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="17">
+      <c r="O8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="16">
         <v>117</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C9" s="18">
+      <c r="C9" s="17">
         <v>41471</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="18">
+      <c r="H9" s="17">
         <v>41564</v>
       </c>
-      <c r="I9" s="16">
-        <v>3</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="17">
+      <c r="I9" s="5">
+        <v>3</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
         <v>33</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="18">
+      <c r="M9" s="17">
         <v>41591</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="5">
         <v>11</v>
       </c>
-      <c r="O9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P9" s="17">
+      <c r="O9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="16">
         <v>126</v>
       </c>
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>41471</v>
       </c>
-      <c r="D10" s="16">
-        <v>3</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17"/>
+      <c r="D10" s="5">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="18">
+      <c r="H10" s="17">
         <v>41564</v>
       </c>
-      <c r="I10" s="16">
-        <v>3</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="17">
+      <c r="I10" s="5">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="16">
         <v>50</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="18">
+      <c r="M10" s="17">
         <v>41591</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="5">
         <v>17</v>
       </c>
-      <c r="O10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="17" t="s">
+      <c r="O10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>27</v>
       </c>
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>41471</v>
       </c>
-      <c r="D11" s="16">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17"/>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="18">
+      <c r="H11" s="17">
         <v>41618</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="5">
         <v>9</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="17">
+      <c r="J11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="16">
         <v>40</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="18">
+      <c r="M11" s="17">
         <v>41591</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="5">
         <v>14</v>
       </c>
-      <c r="O11" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="17" t="s">
+      <c r="O11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="16" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <v>41473</v>
       </c>
-      <c r="D12" s="16">
-        <v>3</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="18">
+      <c r="H12" s="17">
         <v>41618</v>
       </c>
-      <c r="I12" s="16">
-        <v>1</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="17">
+      <c r="I12" s="5">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="16">
         <v>45</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="18">
+      <c r="M12" s="17">
         <v>41591</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="5">
         <v>11</v>
       </c>
-      <c r="O12" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" s="17">
+      <c r="O12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="16">
         <v>122</v>
       </c>
       <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <v>41473</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="5">
         <v>7</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="E13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>41619</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="19">
         <v>8</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="20">
         <v>41</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="18">
+      <c r="M13" s="17">
         <v>41591</v>
       </c>
-      <c r="N13" s="16">
+      <c r="N13" s="5">
         <v>4</v>
       </c>
-      <c r="O13" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="P13" s="17">
+      <c r="O13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" s="16">
         <v>107</v>
       </c>
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>41473</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="E14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="5"/>
@@ -1199,31 +1228,31 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="M14" s="19">
+      <c r="M14" s="18">
         <v>41591</v>
       </c>
-      <c r="N14" s="20">
+      <c r="N14" s="19">
         <v>4</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14" s="21">
+      <c r="O14" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="20">
         <v>115</v>
       </c>
       <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="3:17" ht="30" x14ac:dyDescent="0.3">
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>41473</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>6</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="E15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="5"/>
@@ -1410,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" x14ac:dyDescent="0.25"/>
@@ -2286,4 +2315,913 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CD60BB-7B90-784F-98D7-90E40A97DC51}">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>37</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>48</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="23">
+        <v>41471</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="23">
+        <v>41471</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23">
+        <v>41471</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="23">
+        <v>41471</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="23">
+        <v>41473</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>40</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="23">
+        <v>41473</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>48</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="23">
+        <v>41473</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>29</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="23">
+        <v>41473</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>37</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="23">
+        <v>41647</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>44</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="23">
+        <v>41647</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>45</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="23">
+        <v>41648</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>40</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="23">
+        <v>41648</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>36</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="23">
+        <v>41678</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>52</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="23">
+        <v>41711</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>51</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="23">
+        <v>41711</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>44</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>52</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="23">
+        <v>41505</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>52</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="23">
+        <v>41564</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>33</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="23">
+        <v>41564</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="23">
+        <v>41618</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>40</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="23">
+        <v>41618</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>45</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="23">
+        <v>41619</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>41</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>35</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="23">
+        <v>41590</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>117</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="23">
+        <v>41591</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>126</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="23">
+        <v>41591</v>
+      </c>
+      <c r="C30">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>132</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="23">
+        <v>41591</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>113</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="23">
+        <v>41591</v>
+      </c>
+      <c r="C32">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>122</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="23">
+        <v>41591</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>107</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="23">
+        <v>41591</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>115</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="23">
+        <v>41647</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>157</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="23">
+        <v>41711</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>146</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="23">
+        <v>41647</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="23">
+        <v>41688</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>218</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="23">
+        <v>42102</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="23">
+        <v>42142</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>182</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="23">
+        <v>42193</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>115</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="23">
+        <v>42193</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>190</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="23">
+        <v>41647</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="23">
+        <v>42164</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>29</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="23">
+        <v>41647</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>7</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="23">
+        <v>41688</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>7</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="23">
+        <v>42074</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="23">
+        <v>41647</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>